<commit_message>
add jacobi, knn, stencil
</commit_message>
<xml_diff>
--- a/plot/result.xlsx
+++ b/plot/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23542" windowHeight="12705"/>
+    <workbookView windowWidth="23542" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>us</t>
   </si>
@@ -48,16 +48,25 @@
   <si>
     <t>nw</t>
   </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>stencil</t>
+  </si>
+  <si>
+    <t>jacobi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -69,14 +78,76 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -92,7 +163,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,17 +192,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -124,14 +210,6 @@
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -142,75 +220,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -221,121 +230,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,61 +398,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,9 +426,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -429,6 +440,54 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -462,207 +521,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -670,6 +679,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -991,10 +1006,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.1" outlineLevelCol="7"/>
@@ -1461,8 +1476,235 @@
         <v>63717</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(C20:G20)</f>
         <v>63718.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>877480</v>
+      </c>
+      <c r="D21" s="2">
+        <v>876303</v>
+      </c>
+      <c r="E21" s="1">
+        <v>873813</v>
+      </c>
+      <c r="F21" s="2">
+        <v>873356</v>
+      </c>
+      <c r="G21" s="1">
+        <v>874718</v>
+      </c>
+      <c r="H21">
+        <f>AVERAGE(C21:G21)</f>
+        <v>875134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10530134</v>
+      </c>
+      <c r="D22" s="1">
+        <v>10596535</v>
+      </c>
+      <c r="E22" s="1">
+        <v>10488125</v>
+      </c>
+      <c r="F22" s="1">
+        <v>10838660</v>
+      </c>
+      <c r="G22" s="1">
+        <v>10514119</v>
+      </c>
+      <c r="H22">
+        <f>AVERAGE(C22:G22)</f>
+        <v>10593514.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>269899</v>
+      </c>
+      <c r="D23" s="1">
+        <v>268189</v>
+      </c>
+      <c r="E23" s="1">
+        <v>268547</v>
+      </c>
+      <c r="F23" s="3">
+        <v>268260</v>
+      </c>
+      <c r="G23" s="1">
+        <v>268855</v>
+      </c>
+      <c r="H23">
+        <f>AVERAGE(C23:G23)</f>
+        <v>268750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>734763754</v>
+      </c>
+      <c r="D24">
+        <v>763953191</v>
+      </c>
+      <c r="E24" s="2">
+        <v>728661279</v>
+      </c>
+      <c r="F24" s="2">
+        <v>769087985</v>
+      </c>
+      <c r="G24" s="2">
+        <v>703176758</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H29" si="1">AVERAGE(C24:G24)</f>
+        <v>739928593.4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>896588898</v>
+      </c>
+      <c r="D25">
+        <v>896377042</v>
+      </c>
+      <c r="E25">
+        <v>900184362</v>
+      </c>
+      <c r="F25">
+        <v>900135709</v>
+      </c>
+      <c r="G25" s="2">
+        <v>900031541</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>898663510.4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>98274525</v>
+      </c>
+      <c r="D26">
+        <v>99073909</v>
+      </c>
+      <c r="E26" s="2">
+        <v>98207974</v>
+      </c>
+      <c r="F26">
+        <v>98182549</v>
+      </c>
+      <c r="G26" s="2">
+        <v>101455072</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>99038805.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>19643710</v>
+      </c>
+      <c r="D27" s="2">
+        <v>19603686</v>
+      </c>
+      <c r="E27" s="2">
+        <v>19664439</v>
+      </c>
+      <c r="F27" s="2">
+        <v>19712886</v>
+      </c>
+      <c r="G27" s="2">
+        <v>19589613</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>19642866.8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>67291010</v>
+      </c>
+      <c r="D28" s="2">
+        <v>67301930</v>
+      </c>
+      <c r="E28" s="2">
+        <v>67327774</v>
+      </c>
+      <c r="F28" s="2">
+        <v>67298262</v>
+      </c>
+      <c r="G28" s="2">
+        <v>67293801</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>67302555.4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>398293</v>
+      </c>
+      <c r="D29" s="2">
+        <v>397833</v>
+      </c>
+      <c r="E29" s="2">
+        <v>397831</v>
+      </c>
+      <c r="F29" s="4">
+        <v>398436</v>
+      </c>
+      <c r="G29" s="2">
+        <v>399076</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>398293.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>